<commit_message>
Test de pandas con xlsxwriter para la generación de casos de prueba
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -14,12 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Hello</t>
-  </si>
-  <si>
-    <t>World</t>
+    <t>Data</t>
   </si>
 </sst>
 </file>
@@ -51,12 +48,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -65,7 +77,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,30 +374,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
+      <c r="A2">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>123</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>123.456</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creación de tabla de pruebas y generación de nuevo tests.xlsx
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -14,9 +14,120 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Data</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+  <si>
+    <t>Alé Palacios</t>
+  </si>
+  <si>
+    <t>Gata Fernández</t>
+  </si>
+  <si>
+    <t>Biedma Fresno</t>
+  </si>
+  <si>
+    <t>Yanes Ariza</t>
+  </si>
+  <si>
+    <t>Losada Ostos</t>
+  </si>
+  <si>
+    <t>Merino Verde</t>
+  </si>
+  <si>
+    <t>Benavides Cuevas</t>
+  </si>
+  <si>
+    <t>Francisco</t>
+  </si>
+  <si>
+    <t>José Manuel</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Miguel</t>
+  </si>
+  <si>
+    <t>Guillermo</t>
+  </si>
+  <si>
+    <t>Enrique</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>fraalepal</t>
+  </si>
+  <si>
+    <t>josgatfer</t>
+  </si>
+  <si>
+    <t>pedbiefre</t>
+  </si>
+  <si>
+    <t>migyanari</t>
+  </si>
+  <si>
+    <t>guilosost</t>
+  </si>
+  <si>
+    <t>enrmerver</t>
+  </si>
+  <si>
+    <t>davbencue</t>
+  </si>
+  <si>
+    <t>fraalepal@us.es</t>
+  </si>
+  <si>
+    <t>josgatfer@us.es</t>
+  </si>
+  <si>
+    <t>pedbiefre@us.es</t>
+  </si>
+  <si>
+    <t>migyanari@us.es</t>
+  </si>
+  <si>
+    <t>guilosost@us.es</t>
+  </si>
+  <si>
+    <t>enrmerver@us.es</t>
+  </si>
+  <si>
+    <t>davbencue@us.es</t>
+  </si>
+  <si>
+    <t>http://evidentia.test/20/profiles/view/1</t>
+  </si>
+  <si>
+    <t>http://evidentia.test/20/profiles/view/2</t>
+  </si>
+  <si>
+    <t>http://evidentia.test/20/profiles/view/3</t>
+  </si>
+  <si>
+    <t>http://evidentia.test/20/profiles/view/4</t>
+  </si>
+  <si>
+    <t>http://evidentia.test/20/profiles/view/5</t>
+  </si>
+  <si>
+    <t>http://evidentia.test/20/profiles/view/6</t>
+  </si>
+  <si>
+    <t>http://evidentia.test/20/profiles/view/7</t>
+  </si>
+  <si>
+    <t>ASSISTANCE</t>
+  </si>
+  <si>
+    <t>Sostenibilidad</t>
+  </si>
+  <si>
+    <t>Logística</t>
   </si>
 </sst>
 </file>
@@ -32,12 +143,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -48,7 +158,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -56,32 +166,20 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -374,53 +472,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:18">
+      <c r="A1">
+        <v>111111111</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="R1">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:18">
       <c r="A2">
+        <v>111111112</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+      <c r="R2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:18">
       <c r="A3">
+        <v>111111113</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>10</v>
+      </c>
+      <c r="R3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4">
+        <v>111111114</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4">
+        <v>7</v>
+      </c>
+      <c r="L4">
+        <v>7</v>
+      </c>
+      <c r="R4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5">
+        <v>111111115</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5">
+        <v>10</v>
+      </c>
+      <c r="L5">
+        <v>10</v>
+      </c>
+      <c r="R5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6">
+        <v>111111116</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="R6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7">
+        <v>111111117</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8">
-        <v>45</v>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7">
+        <v>10</v>
+      </c>
+      <c r="L7">
+        <v>10</v>
+      </c>
+      <c r="R7">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F1" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId2"/>
+    <hyperlink ref="F3" r:id="rId3"/>
+    <hyperlink ref="F4" r:id="rId4"/>
+    <hyperlink ref="F5" r:id="rId5"/>
+    <hyperlink ref="F6" r:id="rId6"/>
+    <hyperlink ref="F7" r:id="rId7"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Comprobación de que la casilla de nombre se obtiene correctamente
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -14,7 +14,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
+  <si>
+    <t>DNI</t>
+  </si>
+  <si>
+    <t>Apellidos</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Uvus</t>
+  </si>
+  <si>
+    <t>Correo</t>
+  </si>
+  <si>
+    <t>Perfil</t>
+  </si>
+  <si>
+    <t>Participación</t>
+  </si>
+  <si>
+    <t>Comité</t>
+  </si>
+  <si>
+    <t>Evidencia aleatoria</t>
+  </si>
+  <si>
+    <t>Horas de evidencia aleatoria</t>
+  </si>
+  <si>
+    <t>Eventos asistidos</t>
+  </si>
+  <si>
+    <t>Horas de asistencia</t>
+  </si>
+  <si>
+    <t>Reuniones asistidas</t>
+  </si>
+  <si>
+    <t>Bono de horas</t>
+  </si>
+  <si>
+    <t>Horas de reuniones</t>
+  </si>
+  <si>
+    <t>Evidencias registradas</t>
+  </si>
+  <si>
+    <t>Horas de evidencias</t>
+  </si>
+  <si>
+    <t>Horas en total</t>
+  </si>
   <si>
     <t>Alé Palacios</t>
   </si>
@@ -134,8 +188,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -158,7 +220,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -166,17 +228,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -472,65 +552,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1">
-        <v>111111111</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-      <c r="L1">
-        <v>10</v>
-      </c>
-      <c r="R1">
-        <v>10</v>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2">
-        <v>111111112</v>
+        <v>111111111</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="K2">
         <v>10</v>
@@ -544,28 +648,25 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3">
-        <v>111111113</v>
+        <v>111111112</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="K3">
         <v>10</v>
@@ -579,147 +680,182 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4">
-        <v>111111114</v>
+        <v>111111113</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>53</v>
+      </c>
+      <c r="H4" t="s">
+        <v>54</v>
       </c>
       <c r="K4">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L4">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="R4">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="A5">
-        <v>111111115</v>
+        <v>111111114</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="K5">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L5">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="R5">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="A6">
-        <v>111111116</v>
+        <v>111111115</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>53</v>
+      </c>
+      <c r="H6" t="s">
+        <v>55</v>
       </c>
       <c r="K6">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="L6">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="R6">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="A7">
+        <v>111111116</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="R7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8">
         <v>111111117</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" t="s">
-        <v>37</v>
-      </c>
-      <c r="K7">
-        <v>10</v>
-      </c>
-      <c r="L7">
-        <v>10</v>
-      </c>
-      <c r="R7">
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8">
+        <v>10</v>
+      </c>
+      <c r="L8">
+        <v>10</v>
+      </c>
+      <c r="R8">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F1" r:id="rId1"/>
-    <hyperlink ref="F2" r:id="rId2"/>
-    <hyperlink ref="F3" r:id="rId3"/>
-    <hyperlink ref="F4" r:id="rId4"/>
-    <hyperlink ref="F5" r:id="rId5"/>
-    <hyperlink ref="F6" r:id="rId6"/>
-    <hyperlink ref="F7" r:id="rId7"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F6" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>